<commit_message>
docs: add MIT license with liability waiver and updated the project schedule
</commit_message>
<xml_diff>
--- a/project_schedule.xlsx
+++ b/project_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quadribakre/Documents/project-afara/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C47208-95CB-654C-A4EA-D8ED8351FC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7584F035-09B7-5B45-9813-37F04648525B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="680" windowWidth="24980" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="79">
   <si>
     <t>Device Name</t>
   </si>
@@ -206,23 +206,65 @@
     <t>admin</t>
   </si>
   <si>
-    <t>P521P@s5w0rd</t>
-  </si>
-  <si>
-    <t>Cisco123!</t>
-  </si>
-  <si>
     <t>Test_Rack</t>
   </si>
   <si>
-    <t>Equ!ppd2025!</t>
+    <t>PDU-01</t>
+  </si>
+  <si>
+    <t>PDU-02</t>
+  </si>
+  <si>
+    <t>RMS-01</t>
+  </si>
+  <si>
+    <t>SKY-01</t>
+  </si>
+  <si>
+    <t>SKY-02</t>
+  </si>
+  <si>
+    <t>SKY-03</t>
+  </si>
+  <si>
+    <t>APPLE-01</t>
+  </si>
+  <si>
+    <t>APPLE-02</t>
+  </si>
+  <si>
+    <t>APPLE-03</t>
+  </si>
+  <si>
+    <t>10.20.30.80</t>
+  </si>
+  <si>
+    <t>10.20.30.81</t>
+  </si>
+  <si>
+    <t>10.23.30.120</t>
+  </si>
+  <si>
+    <t>10.23.30.121</t>
+  </si>
+  <si>
+    <t>10.23.30.122</t>
+  </si>
+  <si>
+    <t>10.20.30.130</t>
+  </si>
+  <si>
+    <t>10.20.30.131</t>
+  </si>
+  <si>
+    <t>10.20.30.132</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +276,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -260,7 +308,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -574,7 +622,7 @@
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="21" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="35.33203125" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" customWidth="1"/>
@@ -592,7 +640,7 @@
       <c r="C1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>59</v>
       </c>
       <c r="E1" t="s">
@@ -613,7 +661,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -621,10 +669,7 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="G2" t="s">
@@ -647,9 +692,6 @@
       <c r="C3" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
@@ -676,9 +718,6 @@
       <c r="C4" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
@@ -765,6 +804,10 @@
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="1"/>
       <c r="E8" t="s">
         <v>18</v>
       </c>
@@ -785,6 +828,10 @@
       <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" t="s">
         <v>18</v>
       </c>
@@ -805,6 +852,10 @@
       <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="E10" t="s">
         <v>18</v>
       </c>
@@ -825,6 +876,10 @@
       <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="1"/>
       <c r="E11" t="s">
         <v>18</v>
       </c>
@@ -845,6 +900,10 @@
       <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1"/>
       <c r="E12" t="s">
         <v>18</v>
       </c>
@@ -865,6 +924,10 @@
       <c r="B13" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="1"/>
       <c r="E13" t="s">
         <v>18</v>
       </c>
@@ -885,6 +948,10 @@
       <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="1"/>
       <c r="E14" t="s">
         <v>18</v>
       </c>
@@ -905,6 +972,10 @@
       <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="1"/>
       <c r="E15" t="s">
         <v>18</v>
       </c>
@@ -925,6 +996,10 @@
       <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="1"/>
       <c r="E16" t="s">
         <v>18</v>
       </c>
@@ -945,12 +1020,10 @@
       <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="D17" s="1"/>
       <c r="E17" t="s">
         <v>8</v>
       </c>
@@ -971,12 +1044,10 @@
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="D18" s="1"/>
       <c r="E18" t="s">
         <v>8</v>
       </c>
@@ -997,12 +1068,10 @@
       <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="D19" s="1"/>
       <c r="E19" t="s">
         <v>8</v>
       </c>
@@ -1023,12 +1092,10 @@
       <c r="B20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="D20" s="1"/>
       <c r="E20" t="s">
         <v>8</v>
       </c>
@@ -1049,12 +1116,10 @@
       <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="D21" s="1"/>
       <c r="E21" t="s">
         <v>8</v>
       </c>
@@ -1070,13 +1135,15 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>55</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="G22" t="s">
         <v>9</v>
@@ -1085,6 +1152,180 @@
         <v>10</v>
       </c>
       <c r="I22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="1"/>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Maintenance: Remove legacy Gude driver and update Project Schedule
- Removed 'drivers/gude_pdu.py': Deprecated in favor of the new 'drivers/gude_driver.py'.
- Updated 'project_schedule.xlsx': Added new IP addresses and driver assignments for Commissioning.
</commit_message>
<xml_diff>
--- a/project_schedule.xlsx
+++ b/project_schedule.xlsx
@@ -1,27 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quadribakre/Documents/project-afara/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4BC36D-A9DD-264D-B525-DC73BF3A2130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69521850-E2B5-394C-9775-5026BA83DD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="680" windowWidth="24980" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4420" yWindow="680" windowWidth="24980" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Project Info" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="140">
   <si>
     <t>Device Name</t>
   </si>
@@ -284,12 +299,6 @@
     <t>RMS</t>
   </si>
   <si>
-    <t>CP-01</t>
-  </si>
-  <si>
-    <t>192.168.1.10</t>
-  </si>
-  <si>
     <t>Control</t>
   </si>
   <si>
@@ -314,9 +323,6 @@
     <t>Address</t>
   </si>
   <si>
-    <t>123 Tech Lane, London</t>
-  </si>
-  <si>
     <t>Engineer</t>
   </si>
   <si>
@@ -326,20 +332,137 @@
     <t>Mode</t>
   </si>
   <si>
-    <t>Onsite</t>
-  </si>
-  <si>
-    <t>Afara Project House</t>
-  </si>
-  <si>
-    <t>AFARA-01</t>
+    <t>Offsite</t>
+  </si>
+  <si>
+    <t>TV Room</t>
+  </si>
+  <si>
+    <t>Stevie's Study</t>
+  </si>
+  <si>
+    <t>Gym</t>
+  </si>
+  <si>
+    <t>Dougal's Bedroom</t>
+  </si>
+  <si>
+    <t>Pantry</t>
+  </si>
+  <si>
+    <t>Eaves Storage</t>
+  </si>
+  <si>
+    <t>P521P@s5w0rd</t>
+  </si>
+  <si>
+    <t>gude</t>
+  </si>
+  <si>
+    <t>NVR-01</t>
+  </si>
+  <si>
+    <t>10.21.30.11</t>
+  </si>
+  <si>
+    <t>P521S3curem3</t>
+  </si>
+  <si>
+    <t>NAX-01</t>
+  </si>
+  <si>
+    <t>NAX-02</t>
+  </si>
+  <si>
+    <t>NAX-03</t>
+  </si>
+  <si>
+    <t>NAX-04</t>
+  </si>
+  <si>
+    <t>10.20.30.100</t>
+  </si>
+  <si>
+    <t>10.20.30.101</t>
+  </si>
+  <si>
+    <t>10.20.30.102</t>
+  </si>
+  <si>
+    <t>10.20.30.103</t>
+  </si>
+  <si>
+    <t>Crestron</t>
+  </si>
+  <si>
+    <t>Samsung123</t>
+  </si>
+  <si>
+    <t>Office_Test_Switch</t>
+  </si>
+  <si>
+    <t>Equ!ppd2025!</t>
+  </si>
+  <si>
+    <t>Office_Router</t>
+  </si>
+  <si>
+    <t>192.168.1.1</t>
+  </si>
+  <si>
+    <t>router_draytek</t>
+  </si>
+  <si>
+    <t>v66jU&gt;p3"#eTT</t>
+  </si>
+  <si>
+    <t>v66jU^p3"#eTT</t>
+  </si>
+  <si>
+    <t>C990C@f0j5eq!</t>
+  </si>
+  <si>
+    <t>S9f1wTF8i!k</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>10.20.33.100</t>
+  </si>
+  <si>
+    <t>10.20.33.101</t>
+  </si>
+  <si>
+    <t>gude_driver</t>
+  </si>
+  <si>
+    <t>Afara</t>
+  </si>
+  <si>
+    <t>Afara-01</t>
+  </si>
+  <si>
+    <t>Afara_Dev</t>
+  </si>
+  <si>
+    <t>10.20.30.50</t>
+  </si>
+  <si>
+    <t>CP4-R-Processor</t>
+  </si>
+  <si>
+    <t>TS-770-Kitchen</t>
+  </si>
+  <si>
+    <t>10.20.30.65</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +495,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444746"/>
+      <name val="Google Sans Text"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -393,12 +528,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,13 +837,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -720,7 +856,7 @@
     <col min="10" max="10" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -752,24 +888,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>76</v>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" t="s">
-        <v>78</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
       <c r="E2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" t="s">
-        <v>82</v>
+        <v>132</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -784,21 +916,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
       <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>82</v>
+        <v>132</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
       </c>
       <c r="H3" t="s">
         <v>8</v>
@@ -810,21 +944,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>124</v>
       </c>
       <c r="F4" t="s">
         <v>82</v>
@@ -842,24 +976,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" t="s">
-        <v>52</v>
+        <v>120</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" t="s">
-        <v>82</v>
+      <c r="F5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
       </c>
       <c r="H5" t="s">
         <v>8</v>
@@ -871,18 +1008,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>49</v>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>76</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
         <v>82</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
       </c>
       <c r="H6" t="s">
         <v>8</v>
@@ -894,169 +1040,180 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E11" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F11" t="s">
         <v>83</v>
       </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H11" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="1"/>
       <c r="E12" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>82</v>
+      <c r="F12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
       </c>
       <c r="H12" t="s">
         <v>8</v>
       </c>
       <c r="I12" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>34</v>
@@ -1071,6 +1228,9 @@
       <c r="F13" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
       <c r="H13" t="s">
         <v>8</v>
       </c>
@@ -1078,12 +1238,12 @@
         <v>9</v>
       </c>
       <c r="J13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>34</v>
@@ -1098,6 +1258,9 @@
       <c r="F14" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
       <c r="H14" t="s">
         <v>8</v>
       </c>
@@ -1105,15 +1268,15 @@
         <v>9</v>
       </c>
       <c r="J14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>57</v>
@@ -1125,6 +1288,9 @@
       <c r="F15" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
       <c r="H15" t="s">
         <v>8</v>
       </c>
@@ -1132,15 +1298,15 @@
         <v>9</v>
       </c>
       <c r="J15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>57</v>
@@ -1152,6 +1318,9 @@
       <c r="F16" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
       <c r="H16" t="s">
         <v>8</v>
       </c>
@@ -1159,15 +1328,15 @@
         <v>9</v>
       </c>
       <c r="J16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>57</v>
@@ -1179,33 +1348,39 @@
       <c r="F17" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
       <c r="H17" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="I17" t="s">
         <v>9</v>
       </c>
       <c r="J17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
       <c r="H18" t="s">
         <v>8</v>
       </c>
@@ -1213,25 +1388,28 @@
         <v>9</v>
       </c>
       <c r="J18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>82</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
       </c>
       <c r="H19" t="s">
         <v>8</v>
@@ -1243,22 +1421,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>82</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
       </c>
       <c r="H20" t="s">
         <v>8</v>
@@ -1270,25 +1451,28 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
       <c r="H21" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="I21" t="s">
         <v>9</v>
@@ -1297,23 +1481,28 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="E22" t="s">
         <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
       <c r="H22" t="s">
         <v>8</v>
       </c>
@@ -1324,20 +1513,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
       </c>
       <c r="H23" t="s">
         <v>8</v>
@@ -1349,20 +1545,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
       </c>
       <c r="H24" t="s">
         <v>8</v>
@@ -1374,18 +1577,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
       </c>
       <c r="H25" t="s">
         <v>8</v>
@@ -1397,20 +1609,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="E26" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
       </c>
       <c r="H26" t="s">
         <v>8</v>
@@ -1422,20 +1641,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
       <c r="D27" s="1"/>
       <c r="E27" t="s">
         <v>17</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
       </c>
       <c r="H27" t="s">
         <v>8</v>
@@ -1447,12 +1667,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1460,7 +1680,10 @@
         <v>17</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
       </c>
       <c r="H28" t="s">
         <v>8</v>
@@ -1472,12 +1695,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1485,7 +1708,10 @@
         <v>17</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
       </c>
       <c r="H29" t="s">
         <v>8</v>
@@ -1497,20 +1723,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
       <c r="E30" t="s">
         <v>17</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
       </c>
       <c r="H30" t="s">
         <v>8</v>
@@ -1522,20 +1751,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
       <c r="E31" t="s">
         <v>17</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
       </c>
       <c r="H31" t="s">
         <v>8</v>
@@ -1547,21 +1779,192 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>8</v>
+      </c>
+      <c r="I33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>8</v>
+      </c>
+      <c r="I34" t="s">
+        <v>9</v>
+      </c>
+      <c r="J34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" t="s">
+        <v>105</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C32" t="s">
-        <v>57</v>
-      </c>
-      <c r="F32" t="s">
-        <v>89</v>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>8</v>
+      </c>
+      <c r="I35" t="s">
+        <v>9</v>
+      </c>
+      <c r="J35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" t="s">
+        <v>105</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" t="s">
+        <v>9</v>
+      </c>
+      <c r="J36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>8</v>
+      </c>
+      <c r="I37" t="s">
+        <v>9</v>
+      </c>
+      <c r="J37" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1570,123 +1973,1491 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463240BB-A936-D445-8C9A-309EDCA29A6B}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="52.1640625" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="B3" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="B4" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="4" t="s">
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{611798E3-780D-7543-86CA-083F9008823D}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="6" width="35.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="26.5" customWidth="1"/>
+    <col min="10" max="10" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82AF660-2395-644C-9F79-EB2B2718F180}">
+  <dimension ref="A1:J53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="6" width="35.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="26.5" customWidth="1"/>
+    <col min="10" max="10" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" t="s">
+        <v>106</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="1"/>
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>8</v>
+      </c>
+      <c r="I28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" t="s">
+        <v>82</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>82</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>8</v>
+      </c>
+      <c r="I33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" t="s">
+        <v>9</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" t="s">
+        <v>132</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>8</v>
+      </c>
+      <c r="I37" t="s">
+        <v>9</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" t="s">
+        <v>124</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" t="s">
+        <v>9</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>8</v>
+      </c>
+      <c r="I39" t="s">
+        <v>9</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="s">
+        <v>8</v>
+      </c>
+      <c r="I40" t="s">
+        <v>9</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="s">
+        <v>8</v>
+      </c>
+      <c r="I41" t="s">
+        <v>9</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="F44" s="1"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="F45" s="1"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="F46" s="1"/>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>